<commit_message>
improvements save while running
backup before trying parallel
</commit_message>
<xml_diff>
--- a/tryingAmerican/2015-1-12.xlsx
+++ b/tryingAmerican/2015-1-12.xlsx
@@ -97,6 +97,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,14 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -480,13 +484,15 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -572,22 +578,22 @@
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>20.156110935495899</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>10.996450101614</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>4.6918586420206001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>2.6164755188527602</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>1.44294857205604</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <f>SQRT(0.2*SUM(K8:O8))</f>
         <v>9.8363451255696219E-2</v>
       </c>
@@ -619,23 +625,23 @@
       <c r="A9" s="3">
         <v>2</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>19.861306123434201</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>11.179404404956699</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>5.1285202237821297</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>2.3690579912904401</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>0.99749061188211796</v>
       </c>
-      <c r="G9" s="6">
-        <f t="shared" ref="G9:G10" si="1">SQRT(0.2*SUM(K9:O9))</f>
+      <c r="G9" s="7">
+        <f t="shared" ref="G9:G11" si="1">SQRT(0.2*SUM(K9:O9))</f>
         <v>0.10242833402458679</v>
       </c>
       <c r="H9" s="4">
@@ -666,22 +672,22 @@
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="6">
         <v>19.8629049214132</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>10.6141458972323</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>5.5445091536047801</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>2.6185844587852101</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>1.2606866921931399</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <f t="shared" si="1"/>
         <v>1.7868521606485558E-2</v>
       </c>
@@ -713,44 +719,59 @@
       <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="6">
+        <v>20.0284149341161</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.9255241845361</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5.5318753351538001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2.6290960532929</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1.25806354698319</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
+        <v>8.1110448968388302E-3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5798.2030000000004</v>
+      </c>
       <c r="K11" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.207730269417813E-6</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.6446130839491819E-5</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.8460089709980661E-5</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2.3599445245446515E-8</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2.4180769632854037E-4</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="3"/>
       <c r="K12" s="5">
         <f t="shared" si="2"/>
@@ -777,34 +798,34 @@
       <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="6">
         <v>19.998699999999999</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>10.981999999999999</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>5.4898999999999996</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>2.6295000000000002</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>1.2387999999999999</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="3"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -837,22 +858,22 @@
       <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="6">
         <v>-6.0885909249641701</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>-2.7872627942457999</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>0.26977454438350001</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="6">
         <v>1.6413625987101099</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="6">
         <v>2.4444880748730999</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="7">
         <f>SQRT(0.2*SUM(K18:O18))</f>
         <v>25.969838523703135</v>
       </c>
@@ -884,23 +905,23 @@
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="6">
         <v>4.6359419673860396</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>3.37159105472118</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>3.2546027666096302</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="6">
         <v>3.4942403237927899</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="6">
         <v>3.8399722075588798</v>
       </c>
-      <c r="G19" s="6">
-        <f t="shared" ref="G19:G20" si="8">SQRT(0.2*SUM(K19:O19))</f>
+      <c r="G19" s="7">
+        <f t="shared" ref="G19:G21" si="8">SQRT(0.2*SUM(K19:O19))</f>
         <v>19.007397742962034</v>
       </c>
       <c r="H19" s="4">
@@ -931,22 +952,22 @@
       <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="6">
         <v>6.9430109600893103E-2</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>0.555578254148276</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="6">
         <v>1.47179483214708</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="6">
         <v>2.40533361547081</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="6">
         <v>3.0632351796027502</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="7">
         <f t="shared" si="8"/>
         <v>0.16719019348643427</v>
       </c>
@@ -978,44 +999,59 @@
       <c r="A21" s="3">
         <v>4</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="B21" s="6">
+        <v>0.105811790323906</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.55484458141933402</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.3667324235218801</v>
+      </c>
+      <c r="E21" s="6">
+        <v>2.4156734220249998</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3.0614458387465699</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="8"/>
+        <v>7.4797886978733755E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5798.2030000000004</v>
+      </c>
       <c r="K21" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.6769517368854883E-4</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>8.6942652413011245E-3</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>1.5599811107199695E-2</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>1.8192873028704812E-3</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>1.6925606573572919E-3</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>5</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="3"/>
       <c r="K22" s="5">
         <f t="shared" si="9"/>
@@ -1042,12 +1078,12 @@
       <c r="A23" s="3">
         <v>6</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="3"/>
       <c r="K23" s="5">
         <f t="shared" si="9"/>
@@ -1074,22 +1110,22 @@
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="6">
         <v>0.1072</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>0.6119</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="6">
         <v>1.5618000000000001</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="6">
         <v>2.5232999999999999</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="6">
         <v>3.1928000000000001</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="3"/>
     </row>
   </sheetData>

</xml_diff>